<commit_message>
V1.2 - All OK
</commit_message>
<xml_diff>
--- a/evaluation_debug.xlsx
+++ b/evaluation_debug.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AW3"/>
+  <dimension ref="A1:AW2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -686,243 +686,122 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45654.8375134771</v>
+        <v>45656.97892751805</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
+        <v>2</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
         <v>1</v>
       </c>
-      <c r="L2" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" t="n">
-        <v>4</v>
-      </c>
-      <c r="O2" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="R2" t="n">
-        <v>1</v>
-      </c>
-      <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="n">
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
+      <c r="AA2" t="n">
+        <v>1</v>
+      </c>
       <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="inlineStr"/>
       <c r="AD2" t="n">
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr"/>
       <c r="AG2" t="inlineStr"/>
       <c r="AH2" t="inlineStr"/>
-      <c r="AI2" t="inlineStr"/>
+      <c r="AI2" t="n">
+        <v>3</v>
+      </c>
       <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="inlineStr"/>
       <c r="AL2" t="n">
-        <v>4.8</v>
+        <v>5.600000000000001</v>
       </c>
       <c r="AM2" t="inlineStr"/>
       <c r="AN2" t="inlineStr"/>
       <c r="AO2" t="inlineStr"/>
       <c r="AP2" t="inlineStr"/>
       <c r="AQ2" t="n">
-        <v>4.8</v>
+        <v>8.600000000000001</v>
       </c>
       <c r="AR2" t="n">
         <v>0</v>
       </c>
       <c r="AS2" t="n">
-        <v>4.8</v>
+        <v>8.600000000000001</v>
       </c>
       <c r="AT2" t="inlineStr">
         <is>
-          <t>The Persona reveals his/her job related to ensuring guest satisfaction and operational efficiency in hotel industry; The Persona's engaging demeanor projects openness and attentive customer service</t>
+          <t>The opening question was basic, expecting a polite response without eliciting direct job-to-be-done information.</t>
         </is>
       </c>
       <c r="AU2" t="inlineStr">
         <is>
-          <t>Excellent personal rapport management by the Persona; Good engagement strategy from the Persona's side</t>
+          <t>The persona maintained a pleasant demeanor helping to create rapport.; The response was professionally tailored to his work context.</t>
         </is>
       </c>
       <c r="AV2" t="inlineStr">
         <is>
-          <t>More probing, job-related questions needed from the User; Question lacks depth regarding the target's daily tasks and responsibilities</t>
+          <t>The initial question could be more specific or purposive to inquire about the personas's work or experience.</t>
         </is>
       </c>
       <c r="AW2" t="inlineStr">
         <is>
-          <t>Can you elaborate on your typical day ensuring guest satisfaction and operational efficiency?; What are some of the struggles you face in your job?; What progress are you aiming to make in your job?</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>45654.83844796214</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="K3" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N3" t="n">
-        <v>3</v>
-      </c>
-      <c r="O3" t="n">
-        <v>1</v>
-      </c>
-      <c r="P3" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>1</v>
-      </c>
-      <c r="R3" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="S3" t="n">
-        <v>2.45</v>
-      </c>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>2.45</v>
-      </c>
-      <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="inlineStr"/>
-      <c r="AH3" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>7.349999999999999</v>
-      </c>
-      <c r="AJ3" t="inlineStr"/>
-      <c r="AK3" t="inlineStr"/>
-      <c r="AL3" t="n">
-        <v>4.199999999999999</v>
-      </c>
-      <c r="AM3" t="inlineStr"/>
-      <c r="AN3" t="inlineStr"/>
-      <c r="AO3" t="inlineStr"/>
-      <c r="AP3" t="n">
-        <v>0.8999999999999999</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>11.55</v>
-      </c>
-      <c r="AR3" t="n">
-        <v>0.8999999999999999</v>
-      </c>
-      <c r="AS3" t="n">
-        <v>12.45</v>
-      </c>
-      <c r="AT3" t="inlineStr">
-        <is>
-          <t>The Operations Director has been with Urban Hotels Group for 8 years.; The interviewee emphasizes the importance of providing a superior guest experience.</t>
-        </is>
-      </c>
-      <c r="AU3" t="inlineStr">
-        <is>
-          <t>The interviewee expressed his response well with confidence as a sign of expertise.; The question was well-framed and straightforward, offering clear data.</t>
-        </is>
-      </c>
-      <c r="AV3" t="inlineStr">
-        <is>
-          <t>The question could have been deepened to unearth particular insights about the persona's job.; The response was more about the persona's attitude and lacked specific details about their job-to-be-done.</t>
-        </is>
-      </c>
-      <c r="AW3" t="inlineStr">
-        <is>
-          <t>Could you elaborate on some changes that you've implemented in your duration?; What would you say are some of the biggest achievements in your position over the past 8 years?</t>
+          <t>Can you tell me about a recent challenge in digital banking?; What aspects of risk management are you currently focusing on?</t>
         </is>
       </c>
     </row>

</xml_diff>